<commit_message>
Reformatted table for hospitals w/ only last 6 months in predicted columns
</commit_message>
<xml_diff>
--- a/Project2/Reports/TableDeathsByHospital_formatted.xlsx
+++ b/Project2/Reports/TableDeathsByHospital_formatted.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Hospital</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Percent died</t>
+  </si>
+  <si>
+    <t>Predicted percent died for last 6 months (population-adjusted)</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -556,25 +562,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,6 +583,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -905,36 +908,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -943,12 +950,15 @@
       <c r="C2" s="1">
         <v>87</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="E2" s="1">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -957,12 +967,15 @@
       <c r="C3" s="1">
         <v>107</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="E3" s="1">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -971,12 +984,15 @@
       <c r="C4" s="1">
         <v>100</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="E4" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -985,12 +1001,15 @@
       <c r="C5" s="1">
         <v>94</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="E5" s="1">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -999,12 +1018,15 @@
       <c r="C6" s="1">
         <v>115</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="E6" s="1">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -1013,12 +1035,15 @@
       <c r="C7" s="1">
         <v>104</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1.92</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="E7" s="1">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -1027,12 +1052,15 @@
       <c r="C8" s="1">
         <v>105</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>6.67</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="E8" s="1">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -1041,12 +1069,15 @@
       <c r="C9" s="1">
         <v>120</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="E9" s="1">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -1055,12 +1086,15 @@
       <c r="C10" s="1">
         <v>105</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="E10" s="1">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -1069,12 +1103,15 @@
       <c r="C11" s="1">
         <v>100</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="E11" s="1">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -1083,12 +1120,15 @@
       <c r="C12" s="1">
         <v>90</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="E12" s="1">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="1">
@@ -1097,12 +1137,15 @@
       <c r="C13" s="1">
         <v>98</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>4.08</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="E13" s="1">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -1111,12 +1154,15 @@
       <c r="C14" s="1">
         <v>84</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>4.76</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="E14" s="1">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -1125,12 +1171,15 @@
       <c r="C15" s="1">
         <v>103</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="E15" s="1">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -1139,12 +1188,15 @@
       <c r="C16" s="1">
         <v>105</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>2.86</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="E16" s="1">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -1153,12 +1205,15 @@
       <c r="C17" s="1">
         <v>111</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="E17" s="1">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -1167,12 +1222,15 @@
       <c r="C18" s="1">
         <v>93</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>13.98</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="E18" s="1">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
       <c r="B19" s="1">
@@ -1181,12 +1239,15 @@
       <c r="C19" s="1">
         <v>95</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>2.11</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="E19" s="1">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="1">
@@ -1195,12 +1256,15 @@
       <c r="C20" s="1">
         <v>113</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="E20" s="1">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="1">
@@ -1209,12 +1273,15 @@
       <c r="C21" s="1">
         <v>98</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>2.04</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="E21" s="1">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="1">
@@ -1223,12 +1290,15 @@
       <c r="C22" s="1">
         <v>92</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>5.43</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="E22" s="1">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
       <c r="B23" s="1">
@@ -1237,12 +1307,15 @@
       <c r="C23" s="1">
         <v>86</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>2.33</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="E23" s="1">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="1">
@@ -1251,12 +1324,15 @@
       <c r="C24" s="1">
         <v>97</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>6.19</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="E24" s="1">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
       <c r="B25" s="1">
@@ -1265,12 +1341,15 @@
       <c r="C25" s="1">
         <v>104</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="E25" s="1">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="B26" s="1">
@@ -1279,12 +1358,15 @@
       <c r="C26" s="1">
         <v>96</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>4.17</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="E26" s="1">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
       <c r="B27" s="1">
@@ -1293,12 +1375,15 @@
       <c r="C27" s="1">
         <v>99</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>4.04</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="E27" s="1">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
       <c r="B28" s="1">
@@ -1307,12 +1392,15 @@
       <c r="C28" s="1">
         <v>99</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="E28" s="1">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
       <c r="B29" s="1">
@@ -1321,12 +1409,15 @@
       <c r="C29" s="1">
         <v>101</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>4.95</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="E29" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
       <c r="B30" s="1">
@@ -1335,12 +1426,15 @@
       <c r="C30" s="1">
         <v>105</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="E30" s="1">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
       <c r="B31" s="1">
@@ -1349,12 +1443,15 @@
       <c r="C31" s="1">
         <v>117</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>8.5500000000000007</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>31</v>
       </c>
       <c r="B32" s="1">
@@ -1363,12 +1460,15 @@
       <c r="C32" s="1">
         <v>104</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>6.73</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="E32" s="1">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
       <c r="B33" s="1">
@@ -1377,12 +1477,15 @@
       <c r="C33" s="1">
         <v>93</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="E33" s="1">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <v>33</v>
       </c>
       <c r="B34" s="1">
@@ -1391,12 +1494,15 @@
       <c r="C34" s="1">
         <v>113</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="E34" s="1">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
         <v>34</v>
       </c>
       <c r="B35" s="1">
@@ -1405,12 +1511,15 @@
       <c r="C35" s="1">
         <v>99</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>14.14</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="E35" s="1">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>35</v>
       </c>
       <c r="B36" s="1">
@@ -1419,12 +1528,15 @@
       <c r="C36" s="1">
         <v>84</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>5.95</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="E36" s="1">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
         <v>36</v>
       </c>
       <c r="B37" s="1">
@@ -1433,12 +1545,15 @@
       <c r="C37" s="1">
         <v>99</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <v>1.01</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="E37" s="1">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
         <v>37</v>
       </c>
       <c r="B38" s="1">
@@ -1447,12 +1562,15 @@
       <c r="C38" s="1">
         <v>107</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>3.74</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="E38" s="1">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
         <v>38</v>
       </c>
       <c r="B39" s="1">
@@ -1461,12 +1579,15 @@
       <c r="C39" s="1">
         <v>113</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="E39" s="1">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
         <v>39</v>
       </c>
       <c r="B40" s="1">
@@ -1475,12 +1596,15 @@
       <c r="C40" s="1">
         <v>101</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>3.96</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
         <v>40</v>
       </c>
       <c r="B41" s="1">
@@ -1489,12 +1613,15 @@
       <c r="C41" s="1">
         <v>86</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>2.33</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="E41" s="1">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
         <v>41</v>
       </c>
       <c r="B42" s="1">
@@ -1503,12 +1630,15 @@
       <c r="C42" s="1">
         <v>116</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>4.3099999999999996</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="E42" s="1">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
         <v>42</v>
       </c>
       <c r="B43" s="1">
@@ -1517,12 +1647,15 @@
       <c r="C43" s="1">
         <v>107</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="E43" s="1">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
         <v>43</v>
       </c>
       <c r="B44" s="1">
@@ -1531,25 +1664,32 @@
       <c r="C44" s="1">
         <v>83</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>2.41</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
+      <c r="E44" s="1">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="8">
         <v>0</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="8">
         <v>98</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="8">
         <v>0</v>
+      </c>
+      <c r="E45" s="8">
+        <v>2.99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>